<commit_message>
Implementacion de flujo de investigacion
Se esta realizando la logica del flujo de investigacion
</commit_message>
<xml_diff>
--- a/KavakoWebBot/KavakoWebBotTools/DataPool/Apolo_VendeAuto.xlsx
+++ b/KavakoWebBot/KavakoWebBotTools/DataPool/Apolo_VendeAuto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSUE-CRUZ\source\repos\KavakoWebBot\KavakoWebBotTools\DataPool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSUE-CRUZ\Documents\GitHub\KavakQA\KavakoWebBot\KavakoWebBotTools\DataPool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B304B-5E3C-4063-ACC2-087BFE2AEE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914DB203-4A61-460C-9777-F21F9C6B65AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6885" yWindow="3255" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="128">
   <si>
     <t>ResultadoEsperado</t>
   </si>
@@ -403,13 +403,16 @@
     <t>APOLO - VENDE TU AUTO - 01 - HP</t>
   </si>
   <si>
-    <t>Jueves 27 Febrero</t>
-  </si>
-  <si>
     <t>APOLO - VENDE TU AUTO - 02 - HP</t>
   </si>
   <si>
     <t>APOLO - VENDE TU AUTO - 03 - HP</t>
+  </si>
+  <si>
+    <t>Jueves 05 Marzo</t>
+  </si>
+  <si>
+    <t>Lunes 09 Marzo</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1056,7 @@
     </row>
     <row r="3" spans="1:13 16374:16384" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>92</v>
@@ -1124,7 +1127,7 @@
     </row>
     <row r="4" spans="1:13 16374:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>92</v>
@@ -1414,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XEX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1575,7 @@
         <v>114</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>94</v>
@@ -1637,7 +1640,7 @@
       </c>
       <c r="R3" s="6"/>
       <c r="S3" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>96</v>
@@ -1709,7 +1712,7 @@
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T4" s="6" t="s">
         <v>98</v>
@@ -1781,7 +1784,7 @@
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T5" s="6" t="s">
         <v>102</v>
@@ -1853,7 +1856,7 @@
       </c>
       <c r="R6" s="6"/>
       <c r="S6" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T6" s="6" t="s">
         <v>102</v>
@@ -1925,7 +1928,7 @@
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T7" s="6" t="s">
         <v>104</v>
@@ -1997,7 +2000,7 @@
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T8" s="6" t="s">
         <v>106</v>

</xml_diff>